<commit_message>
Atualização na Planilha de Especificação de Dados com Exemplos
</commit_message>
<xml_diff>
--- a/files/specs/docs/filespecs.xlsx
+++ b/files/specs/docs/filespecs.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel Couto\Documents\repos\BBDataSet\BBDataSet\files\specs\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E58C0A24-F226-4B67-B4E4-A0A714C4D753}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855C0847-FB20-49D3-A2CB-5D24738103C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{7EF4552A-52FB-481D-B5EA-A7BEC44E0E3B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{7EF4552A-52FB-481D-B5EA-A7BEC44E0E3B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Arquivos de Dados" sheetId="1" r:id="rId1"/>
+    <sheet name="Arquivos de Índices" sheetId="2" r:id="rId2"/>
+    <sheet name="Antiga" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,42 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="90">
   <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nome do artista </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weeks on Board do Artista (calculado a partir do Weeks on Board das músicas do artista) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1ª aparição </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Última aparição </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data da melhor
-semana </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quantidade de títulos
- na melhor semana </t>
-  </si>
-  <si>
-    <t>Título</t>
-  </si>
-  <si>
-    <t>Peak Rank</t>
-  </si>
-  <si>
-    <t>Weeks on Board da música</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nome do
- artista  </t>
   </si>
   <si>
     <t xml:space="preserve">Nome </t>
@@ -108,12 +77,6 @@
   </si>
   <si>
     <t>Notas</t>
-  </si>
-  <si>
-    <t>Arquivo 1 - Entidade Artista e Melhor Semana</t>
-  </si>
-  <si>
-    <t>Arquivo 2 - Entidade Música</t>
   </si>
   <si>
     <t xml:space="preserve">indice-artista </t>
@@ -193,9 +156,6 @@
     <t>em que formato a gente vai colocar no arquivo</t>
   </si>
   <si>
-    <t>arquivo tem indice</t>
-  </si>
-  <si>
     <t>tira do csv</t>
   </si>
   <si>
@@ -232,14 +192,190 @@
     <t>duplicata de nome de musica</t>
   </si>
   <si>
-    <t xml:space="preserve">(se não tiver artista, não tem a </t>
+    <t>(se não tiver artista, não tem a NOSSA musica, entao adicionar os dois</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>tem musica e tem artista</t>
+  </si>
+  <si>
+    <t>tem musica e não tem artista</t>
+  </si>
+  <si>
+    <t>não tem musica e tem artista</t>
+  </si>
+  <si>
+    <t>não tem musica nem artista</t>
+  </si>
+  <si>
+    <t>qual verificacao eh mais propria não sei</t>
+  </si>
+  <si>
+    <t>(arquivos binarios tem indice)</t>
+  </si>
+  <si>
+    <t>se já tem artista, substituir primeira aparicao pela data atual</t>
+  </si>
+  <si>
+    <t>colocar data atual, mas sabendo que ta possivelmente errada</t>
+  </si>
+  <si>
+    <t>(supondo priemira ocorrencia do artista, colocar 1 no wob)</t>
+  </si>
+  <si>
+    <t>se já tem artista, incrementar weeks on board, mas vendo se o artista aparece 2 vezes em uma mesma semana</t>
+  </si>
+  <si>
+    <t>para melhor semana:</t>
+  </si>
+  <si>
+    <t>não dá, mas pensa assim: coloca semana no melhor semana. Conforme for passando o tempo, se repete o artista, if data eq data, incremenetar o ocorrencias</t>
+  </si>
+  <si>
+    <t>Título.</t>
+  </si>
+  <si>
+    <t>Peak Rank.</t>
+  </si>
+  <si>
+    <t>Weeks on Board da música.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nome do
+ artista.  </t>
+  </si>
+  <si>
+    <t>Weeks on Board do Artista (calculado a partir do Weeks on Board das músicas do artista).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nome do artista. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1ª aparição. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Última aparição. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data da melhor
+semana. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantidade de títulos
+ na melhor semana. </t>
+  </si>
+  <si>
+    <t>adicionando indices!</t>
+  </si>
+  <si>
+    <t># decidir: se artistIsPresent já retorna os dados. Será usada para o programa principal tbm.</t>
+  </si>
+  <si>
+    <t>e a entidade melhor semana?</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>soma de dpos valores</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>Exibição 1 
+para Usuário</t>
+  </si>
+  <si>
+    <t>Exibição 2 
+para Usuário</t>
+  </si>
+  <si>
+    <t>Arquivo de Dados 1 - Entidade Artista e Melhor Semana</t>
+  </si>
+  <si>
+    <t>Arquivo de Dados 2 - Entidade Música</t>
+  </si>
+  <si>
+    <t>Arquivo de Índice 1</t>
+  </si>
+  <si>
+    <t>Arquivo de Índice 2</t>
+  </si>
+  <si>
+    <t>Arquivo de Índice 3</t>
+  </si>
+  <si>
+    <t>Arquivo de Índice 4</t>
+  </si>
+  <si>
+    <t>Arquivo de Índice n</t>
+  </si>
+  <si>
+    <t>Posição</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID </t>
+  </si>
+  <si>
+    <t>Exemplo de Arquivo de Dados - Entidade Música</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Posição no Arquivo</t>
+  </si>
+  <si>
+    <t>Título</t>
+  </si>
+  <si>
+    <t>Peak Rank</t>
+  </si>
+  <si>
+    <t>indice-
+musica</t>
+  </si>
+  <si>
+    <t>Posição no Arquivo de Dados</t>
+  </si>
+  <si>
+    <t>Exemplo de Arquivo
+ de Índice - Nome da Faixa</t>
+  </si>
+  <si>
+    <t>Exemplo de Arquivo
+ de Índice - Peak Rank</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -259,6 +395,29 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -308,7 +467,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -393,11 +552,70 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -442,27 +660,83 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -777,10 +1051,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88364B05-4AB7-4140-8F17-B06F82EDA48C}">
-  <dimension ref="A1:M29"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -796,24 +1070,24 @@
     <col min="12" max="12" width="4.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="23"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B2" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="20"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -823,233 +1097,1183 @@
       <c r="E3" s="22"/>
       <c r="F3" s="22"/>
       <c r="G3" s="22"/>
-      <c r="H3" s="24"/>
-    </row>
-    <row r="4" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="H3" s="23"/>
+    </row>
+    <row r="4" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" s="29" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="20"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="21"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="23"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="E9" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="29" t="str">
+        <f>H5</f>
+        <v>I</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M12" t="s">
+        <v>0</v>
+      </c>
+      <c r="N12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="23"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I15" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="24"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="13" t="s">
+      <c r="K15" s="11"/>
+      <c r="M15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="K17" s="10"/>
+      <c r="M17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C19" s="48"/>
+      <c r="K19" s="15"/>
+      <c r="M19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="K21" s="12"/>
+      <c r="M21" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K13" s="11"/>
-      <c r="M13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K15" s="10"/>
-      <c r="M15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+    </row>
+    <row r="22" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="J22" t="s">
         <v>0</v>
       </c>
-      <c r="C16" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+    </row>
+    <row r="23" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
         <v>0</v>
       </c>
-      <c r="C17" t="s">
-        <v>32</v>
-      </c>
-      <c r="K17" s="15"/>
-      <c r="M17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+    </row>
+    <row r="29" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="N29" t="s">
         <v>0</v>
       </c>
-      <c r="F18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="G19" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="H19" s="18"/>
-      <c r="I19" t="s">
-        <v>38</v>
-      </c>
-      <c r="K19" s="12"/>
-      <c r="M19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" t="s">
+    </row>
+    <row r="30" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="N30" t="s">
         <v>0</v>
-      </c>
-      <c r="G20" t="s">
-        <v>39</v>
-      </c>
-      <c r="I20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D22" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D23" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D24" t="s">
-        <v>35</v>
-      </c>
-      <c r="E24" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="E25" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D28" t="s">
-        <v>44</v>
-      </c>
-      <c r="E28" t="s">
-        <v>42</v>
-      </c>
-      <c r="F28" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="E29" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B2:H3"/>
-    <mergeCell ref="B6:G7"/>
-    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="B7:G8"/>
+    <mergeCell ref="G21:H21"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9AECEB1-E543-4883-A1BE-73D1011192D9}">
+  <dimension ref="B2:P43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C2" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="20"/>
+      <c r="F2" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" s="20"/>
+      <c r="I2" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" s="20"/>
+      <c r="L2" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="M2" s="20"/>
+      <c r="O2" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="P2" s="20"/>
+    </row>
+    <row r="3" spans="3:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="21"/>
+      <c r="D3" s="23"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="23"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="23"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="23"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="23"/>
+    </row>
+    <row r="4" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="I4" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="J4" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="L4" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="M4" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="O4" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="P4" s="35" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C5" s="39"/>
+      <c r="D5" s="36"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="36"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="36"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="36"/>
+      <c r="O5" s="39"/>
+      <c r="P5" s="36"/>
+    </row>
+    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C6" s="40"/>
+      <c r="D6" s="37"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="37"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="37"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="37"/>
+      <c r="O6" s="40"/>
+      <c r="P6" s="37"/>
+    </row>
+    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C7" s="40"/>
+      <c r="D7" s="37"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="37"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="37"/>
+      <c r="L7" s="40"/>
+      <c r="M7" s="37"/>
+      <c r="O7" s="40"/>
+      <c r="P7" s="37"/>
+    </row>
+    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C8" s="40"/>
+      <c r="D8" s="37"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="37"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="37"/>
+      <c r="L8" s="40"/>
+      <c r="M8" s="37"/>
+      <c r="O8" s="40"/>
+      <c r="P8" s="37"/>
+    </row>
+    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C9" s="40"/>
+      <c r="D9" s="37"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="37"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="37"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="37"/>
+      <c r="O9" s="40"/>
+      <c r="P9" s="37"/>
+    </row>
+    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C10" s="40"/>
+      <c r="D10" s="37"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="37"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="37"/>
+      <c r="L10" s="40"/>
+      <c r="M10" s="37"/>
+      <c r="O10" s="40"/>
+      <c r="P10" s="37"/>
+    </row>
+    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C11" s="40"/>
+      <c r="D11" s="37"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="37"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="37"/>
+      <c r="L11" s="40"/>
+      <c r="M11" s="37"/>
+      <c r="O11" s="40"/>
+      <c r="P11" s="37"/>
+    </row>
+    <row r="12" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C12" s="40"/>
+      <c r="D12" s="37"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="37"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="37"/>
+      <c r="L12" s="40"/>
+      <c r="M12" s="37"/>
+      <c r="O12" s="40"/>
+      <c r="P12" s="37"/>
+    </row>
+    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C13" s="40"/>
+      <c r="D13" s="37"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="37"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="37"/>
+      <c r="L13" s="40"/>
+      <c r="M13" s="37"/>
+      <c r="O13" s="40"/>
+      <c r="P13" s="37"/>
+    </row>
+    <row r="14" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C14" s="40"/>
+      <c r="D14" s="37"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="37"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="37"/>
+      <c r="L14" s="40"/>
+      <c r="M14" s="37"/>
+      <c r="O14" s="40"/>
+      <c r="P14" s="37"/>
+    </row>
+    <row r="15" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C15" s="40"/>
+      <c r="D15" s="37"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="37"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="37"/>
+      <c r="L15" s="40"/>
+      <c r="M15" s="37"/>
+      <c r="O15" s="40"/>
+      <c r="P15" s="37"/>
+    </row>
+    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C16" s="40"/>
+      <c r="D16" s="37"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="37"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="37"/>
+      <c r="L16" s="40"/>
+      <c r="M16" s="37"/>
+      <c r="O16" s="40"/>
+      <c r="P16" s="37"/>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C17" s="40"/>
+      <c r="D17" s="37"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="37"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="37"/>
+      <c r="L17" s="40"/>
+      <c r="M17" s="37"/>
+      <c r="O17" s="40"/>
+      <c r="P17" s="37"/>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C18" s="40"/>
+      <c r="D18" s="37"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="37"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="37"/>
+      <c r="L18" s="40"/>
+      <c r="M18" s="37"/>
+      <c r="O18" s="40"/>
+      <c r="P18" s="37"/>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C19" s="41"/>
+      <c r="D19" s="38"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="38"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="38"/>
+      <c r="L19" s="41"/>
+      <c r="M19" s="38"/>
+      <c r="O19" s="41"/>
+      <c r="P19" s="38"/>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B26" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="J26" s="47" t="s">
+        <v>88</v>
+      </c>
+      <c r="K26" s="20"/>
+      <c r="M26" s="47" t="s">
+        <v>89</v>
+      </c>
+      <c r="N26" s="20"/>
+    </row>
+    <row r="27" spans="2:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="21"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="23"/>
+      <c r="M27" s="21"/>
+      <c r="N27" s="23"/>
+    </row>
+    <row r="28" spans="2:16" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="D28" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="E28" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" s="46" t="s">
+        <v>86</v>
+      </c>
+      <c r="H28" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="J28" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="K28" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="M28" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="N28" s="35" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B29" s="41">
+        <v>0</v>
+      </c>
+      <c r="C29" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="D29" s="42">
+        <v>2</v>
+      </c>
+      <c r="E29" s="42"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="42">
+        <v>675455</v>
+      </c>
+      <c r="H29" s="42"/>
+      <c r="J29" s="39">
+        <v>87585</v>
+      </c>
+      <c r="K29" s="36">
+        <v>2</v>
+      </c>
+      <c r="M29" s="39">
+        <v>32432</v>
+      </c>
+      <c r="N29" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B30" s="42">
+        <v>1</v>
+      </c>
+      <c r="C30" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="D30" s="42">
+        <v>1</v>
+      </c>
+      <c r="E30" s="42"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="42">
+        <v>32432</v>
+      </c>
+      <c r="H30" s="42"/>
+      <c r="J30" s="40">
+        <v>124435</v>
+      </c>
+      <c r="K30" s="37">
+        <v>3</v>
+      </c>
+      <c r="M30" s="40">
+        <v>675455</v>
+      </c>
+      <c r="N30" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B31" s="42">
+        <v>2</v>
+      </c>
+      <c r="C31" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="D31" s="42">
+        <v>7</v>
+      </c>
+      <c r="E31" s="42"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="39">
+        <v>87585</v>
+      </c>
+      <c r="H31" s="42"/>
+      <c r="J31" s="40">
+        <v>32432</v>
+      </c>
+      <c r="K31" s="37">
+        <v>1</v>
+      </c>
+      <c r="M31" s="40">
+        <v>124435</v>
+      </c>
+      <c r="N31" s="37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B32" s="42">
+        <v>3</v>
+      </c>
+      <c r="C32" s="42" t="s">
+        <v>78</v>
+      </c>
+      <c r="D32" s="42">
+        <v>3</v>
+      </c>
+      <c r="E32" s="42"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="42">
+        <v>124435</v>
+      </c>
+      <c r="H32" s="42"/>
+      <c r="J32" s="40">
+        <v>877856</v>
+      </c>
+      <c r="K32" s="37">
+        <v>4</v>
+      </c>
+      <c r="M32" s="40">
+        <v>87585</v>
+      </c>
+      <c r="N32" s="37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B33" s="42">
+        <v>4</v>
+      </c>
+      <c r="C33" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="D33" s="42">
+        <v>9</v>
+      </c>
+      <c r="E33" s="42"/>
+      <c r="F33" s="42"/>
+      <c r="G33" s="42">
+        <v>877856</v>
+      </c>
+      <c r="H33" s="42"/>
+      <c r="J33" s="40">
+        <v>675455</v>
+      </c>
+      <c r="K33" s="37">
+        <v>0</v>
+      </c>
+      <c r="M33" s="40">
+        <v>877856</v>
+      </c>
+      <c r="N33" s="37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B34" s="42">
+        <v>5</v>
+      </c>
+      <c r="C34" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="D34" s="42">
+        <v>15</v>
+      </c>
+      <c r="E34" s="42"/>
+      <c r="F34" s="42"/>
+      <c r="G34" s="42">
+        <v>767567</v>
+      </c>
+      <c r="H34" s="42"/>
+      <c r="J34" s="40">
+        <v>767567</v>
+      </c>
+      <c r="K34" s="37">
+        <v>5</v>
+      </c>
+      <c r="M34" s="40">
+        <v>767567</v>
+      </c>
+      <c r="N34" s="37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="J35" s="40"/>
+      <c r="K35" s="37"/>
+      <c r="M35" s="40"/>
+      <c r="N35" s="37"/>
+    </row>
+    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="J36" s="40"/>
+      <c r="K36" s="37"/>
+      <c r="M36" s="40"/>
+      <c r="N36" s="37"/>
+    </row>
+    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="J37" s="40"/>
+      <c r="K37" s="37"/>
+      <c r="M37" s="40"/>
+      <c r="N37" s="37"/>
+    </row>
+    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="J38" s="40"/>
+      <c r="K38" s="37"/>
+      <c r="M38" s="40"/>
+      <c r="N38" s="37"/>
+    </row>
+    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="J39" s="40"/>
+      <c r="K39" s="37"/>
+      <c r="M39" s="40"/>
+      <c r="N39" s="37"/>
+    </row>
+    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="J40" s="40"/>
+      <c r="K40" s="37"/>
+      <c r="M40" s="40"/>
+      <c r="N40" s="37"/>
+    </row>
+    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="J41" s="40"/>
+      <c r="K41" s="37"/>
+      <c r="M41" s="40"/>
+      <c r="N41" s="37"/>
+    </row>
+    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="J42" s="40"/>
+      <c r="K42" s="37"/>
+      <c r="M42" s="40"/>
+      <c r="N42" s="37"/>
+    </row>
+    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="J43" s="41"/>
+      <c r="K43" s="38"/>
+      <c r="M43" s="41"/>
+      <c r="N43" s="38"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="O2:P3"/>
+    <mergeCell ref="J26:K27"/>
+    <mergeCell ref="B26:H27"/>
+    <mergeCell ref="M26:N27"/>
+    <mergeCell ref="C2:D3"/>
+    <mergeCell ref="F2:G3"/>
+    <mergeCell ref="I2:J3"/>
+    <mergeCell ref="L2:M3"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{263AA3E4-D416-4942-A6CE-1FC6D8EAF08C}">
+  <dimension ref="A1:N37"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B2" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="20"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="21"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="23"/>
+    </row>
+    <row r="4" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" s="29" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="20"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="21"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="23"/>
+    </row>
+    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="29" t="str">
+        <f>H5</f>
+        <v>I</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="195" x14ac:dyDescent="0.25">
+      <c r="A12" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I15" t="s">
+        <v>57</v>
+      </c>
+      <c r="K15" s="11"/>
+      <c r="M15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="K17" s="10"/>
+      <c r="M17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>20</v>
+      </c>
+      <c r="K19" s="15"/>
+      <c r="M19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="G21" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="H21" s="24"/>
+      <c r="I21" t="s">
+        <v>25</v>
+      </c>
+      <c r="K21" s="12"/>
+      <c r="M21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" t="s">
+        <v>0</v>
+      </c>
+      <c r="G22" t="s">
+        <v>26</v>
+      </c>
+      <c r="I22" t="s">
+        <v>27</v>
+      </c>
+      <c r="J22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" t="s">
+        <v>29</v>
+      </c>
+      <c r="G26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>30</v>
+      </c>
+      <c r="I27" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="N29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E30" t="s">
+        <v>29</v>
+      </c>
+      <c r="F30" t="s">
+        <v>33</v>
+      </c>
+      <c r="N30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>35</v>
+      </c>
+      <c r="G34" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>36</v>
+      </c>
+      <c r="G35" t="s">
+        <v>34</v>
+      </c>
+      <c r="H35" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B2:H3"/>
+    <mergeCell ref="B7:G8"/>
+    <mergeCell ref="G21:H21"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>